<commit_message>
alguns pormenores no diagrama
</commit_message>
<xml_diff>
--- a/Fundamentacao/gantt-chart_L2.xlsx
+++ b/Fundamentacao/gantt-chart_L2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joao/Desktop/Desktop_iCloud/Universidade/3ºano/2ºsemestre/LI4/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joao/Desktop/Desktop_iCloud/Universidade/3ºano/2ºsemestre/LI4/MyChef/Fundamentacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBA4282-76E5-2A45-BD6F-40057BA06C2B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4595411-82E0-AA40-AC88-4062FE11CB8B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -481,7 +481,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="156">
   <si>
     <t>WBS</t>
   </si>
@@ -1584,6 +1584,9 @@
   </si>
   <si>
     <t>MyChef - Feel the Italian</t>
+  </si>
+  <si>
+    <t>HOURS</t>
   </si>
 </sst>
 </file>
@@ -2346,7 +2349,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -2840,28 +2843,6 @@
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="FFEFEFEF"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
       </top>
       <bottom style="thin">
@@ -2882,10 +2863,150 @@
       <left/>
       <right/>
       <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
         <color indexed="22"/>
       </top>
       <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFEFEFEF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFEFEFEF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFEFEFEF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFEFEFEF"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFEFEFEF"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFEFEFEF"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2939,7 +3060,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="236">
+  <cellXfs count="247">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3098,9 +3219,6 @@
     <xf numFmtId="9" fontId="40" fillId="22" borderId="11" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="48" fillId="27" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3416,22 +3534,97 @@
     <xf numFmtId="0" fontId="45" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="57" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="40" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="40" fillId="22" borderId="0" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="57" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="40" fillId="22" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="40" fillId="22" borderId="44" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="56" fillId="20" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="23" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="23" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="51" fillId="23" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="51" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="51" fillId="23" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="51" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="51" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="51" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="51" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="51" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="51" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="84" fillId="24" borderId="0" xfId="34" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="70" fillId="23" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="70" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="70" fillId="23" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="51" fillId="23" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="51" fillId="23" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="51" fillId="23" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3479,101 +3672,62 @@
     <xf numFmtId="167" fontId="51" fillId="23" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="70" fillId="23" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="23" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="51" fillId="23" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="51" fillId="23" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="51" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="51" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="51" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="51" fillId="23" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="23" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="23" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="51" fillId="23" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="51" fillId="23" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="61" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="61" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="57" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="40" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="40" fillId="22" borderId="0" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="57" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="61" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="59" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="40" fillId="22" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="40" fillId="22" borderId="46" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="37" fillId="20" borderId="44" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="56" fillId="20" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="59" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="59" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="40" fillId="22" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="40" fillId="22" borderId="50" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="61" fillId="22" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="61" fillId="22" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="61" fillId="22" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="61" fillId="22" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="61" fillId="22" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="60" fillId="20" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="59" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3760,8 +3914,8 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -4407,7 +4561,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -4420,13 +4574,13 @@
     <col min="7" max="7" width="6" style="33" customWidth="1"/>
     <col min="8" max="8" width="6.6640625" style="33" customWidth="1"/>
     <col min="9" max="9" width="5.83203125" style="33" customWidth="1"/>
-    <col min="10" max="10" width="1.5" style="33" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" style="33" customWidth="1"/>
     <col min="11" max="66" width="2.5" style="33" customWidth="1"/>
     <col min="67" max="16384" width="9.1640625" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:150" s="66" customFormat="1" ht="33" customHeight="1">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="154" t="s">
         <v>154</v>
       </c>
       <c r="B1" s="63"/>
@@ -4434,7 +4588,7 @@
       <c r="D1" s="63"/>
       <c r="E1" s="63"/>
       <c r="F1" s="63"/>
-      <c r="G1" s="183"/>
+      <c r="G1" s="182"/>
       <c r="H1" s="64"/>
       <c r="I1" s="64"/>
       <c r="J1" s="64"/>
@@ -4457,21 +4611,21 @@
       <c r="AA1" s="64"/>
       <c r="AB1" s="64"/>
       <c r="AC1" s="64"/>
-      <c r="AD1" s="184"/>
-      <c r="AE1" s="184"/>
-      <c r="AF1" s="184"/>
-      <c r="AG1" s="184"/>
-      <c r="AH1" s="184"/>
-      <c r="AI1" s="184"/>
-      <c r="AJ1" s="184"/>
-      <c r="AK1" s="184"/>
-      <c r="AL1" s="184"/>
-      <c r="AM1" s="184"/>
-      <c r="AN1" s="184"/>
-      <c r="AO1" s="184"/>
-      <c r="AP1" s="184"/>
-      <c r="AQ1" s="184"/>
-      <c r="AR1" s="184"/>
+      <c r="AD1" s="210"/>
+      <c r="AE1" s="210"/>
+      <c r="AF1" s="210"/>
+      <c r="AG1" s="210"/>
+      <c r="AH1" s="210"/>
+      <c r="AI1" s="210"/>
+      <c r="AJ1" s="210"/>
+      <c r="AK1" s="210"/>
+      <c r="AL1" s="210"/>
+      <c r="AM1" s="210"/>
+      <c r="AN1" s="210"/>
+      <c r="AO1" s="210"/>
+      <c r="AP1" s="210"/>
+      <c r="AQ1" s="210"/>
+      <c r="AR1" s="210"/>
       <c r="AS1" s="64"/>
       <c r="AT1" s="64"/>
       <c r="AU1" s="64"/>
@@ -4495,851 +4649,853 @@
       <c r="BM1" s="64"/>
       <c r="BN1" s="64"/>
     </row>
-    <row r="2" spans="1:150" s="89" customFormat="1" ht="21" customHeight="1">
-      <c r="A2" s="149" t="s">
+    <row r="2" spans="1:150" s="88" customFormat="1" ht="21" customHeight="1">
+      <c r="A2" s="148" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="88"/>
-    </row>
-    <row r="3" spans="1:150" s="133" customFormat="1" ht="6.75" customHeight="1" thickBot="1">
-      <c r="A3" s="128"/>
-      <c r="B3" s="129"/>
-      <c r="C3" s="129"/>
-      <c r="D3" s="130"/>
-      <c r="E3" s="131"/>
-      <c r="F3" s="132"/>
-      <c r="K3" s="152"/>
-      <c r="L3" s="153"/>
-      <c r="M3" s="153"/>
-      <c r="N3" s="153"/>
-      <c r="O3" s="153"/>
-      <c r="P3" s="153"/>
-      <c r="Q3" s="154"/>
-      <c r="R3" s="152"/>
-      <c r="S3" s="153"/>
-      <c r="T3" s="153"/>
-      <c r="U3" s="153"/>
-      <c r="V3" s="153"/>
-      <c r="W3" s="153"/>
-      <c r="X3" s="154"/>
-      <c r="Y3" s="152"/>
-      <c r="Z3" s="153"/>
-      <c r="AA3" s="153"/>
-      <c r="AB3" s="153"/>
-      <c r="AC3" s="153"/>
-      <c r="AD3" s="153"/>
-      <c r="AE3" s="154"/>
-      <c r="AF3" s="152"/>
-      <c r="AG3" s="153"/>
-      <c r="AH3" s="153"/>
-      <c r="AI3" s="153"/>
-      <c r="AJ3" s="153"/>
-      <c r="AK3" s="153"/>
-      <c r="AL3" s="154"/>
-      <c r="AM3" s="152"/>
-      <c r="AN3" s="153"/>
-      <c r="AO3" s="153"/>
-      <c r="AP3" s="153"/>
-      <c r="AQ3" s="153"/>
-      <c r="AR3" s="153"/>
-      <c r="AS3" s="154"/>
-      <c r="AT3" s="152"/>
-      <c r="AU3" s="153"/>
-      <c r="AV3" s="153"/>
-      <c r="AW3" s="153"/>
-      <c r="AX3" s="153"/>
-      <c r="AY3" s="153"/>
-      <c r="AZ3" s="154"/>
-      <c r="BA3" s="152"/>
-      <c r="BB3" s="153"/>
-      <c r="BC3" s="153"/>
-      <c r="BD3" s="153"/>
-      <c r="BE3" s="153"/>
-      <c r="BF3" s="153"/>
-      <c r="BG3" s="154"/>
-      <c r="BH3" s="152"/>
-      <c r="BI3" s="153"/>
-      <c r="BJ3" s="153"/>
-      <c r="BK3" s="153"/>
-      <c r="BL3" s="153"/>
-      <c r="BM3" s="153"/>
-      <c r="BN3" s="154"/>
-    </row>
-    <row r="4" spans="1:150" s="145" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A4" s="147"/>
-      <c r="B4" s="150" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="87"/>
+    </row>
+    <row r="3" spans="1:150" s="132" customFormat="1" ht="6.75" customHeight="1" thickBot="1">
+      <c r="A3" s="127"/>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="131"/>
+      <c r="K3" s="151"/>
+      <c r="L3" s="152"/>
+      <c r="M3" s="152"/>
+      <c r="N3" s="152"/>
+      <c r="O3" s="152"/>
+      <c r="P3" s="152"/>
+      <c r="Q3" s="153"/>
+      <c r="R3" s="151"/>
+      <c r="S3" s="152"/>
+      <c r="T3" s="152"/>
+      <c r="U3" s="152"/>
+      <c r="V3" s="152"/>
+      <c r="W3" s="152"/>
+      <c r="X3" s="153"/>
+      <c r="Y3" s="151"/>
+      <c r="Z3" s="152"/>
+      <c r="AA3" s="152"/>
+      <c r="AB3" s="152"/>
+      <c r="AC3" s="152"/>
+      <c r="AD3" s="152"/>
+      <c r="AE3" s="153"/>
+      <c r="AF3" s="151"/>
+      <c r="AG3" s="152"/>
+      <c r="AH3" s="152"/>
+      <c r="AI3" s="152"/>
+      <c r="AJ3" s="152"/>
+      <c r="AK3" s="152"/>
+      <c r="AL3" s="153"/>
+      <c r="AM3" s="151"/>
+      <c r="AN3" s="152"/>
+      <c r="AO3" s="152"/>
+      <c r="AP3" s="152"/>
+      <c r="AQ3" s="152"/>
+      <c r="AR3" s="152"/>
+      <c r="AS3" s="153"/>
+      <c r="AT3" s="151"/>
+      <c r="AU3" s="152"/>
+      <c r="AV3" s="152"/>
+      <c r="AW3" s="152"/>
+      <c r="AX3" s="152"/>
+      <c r="AY3" s="152"/>
+      <c r="AZ3" s="153"/>
+      <c r="BA3" s="151"/>
+      <c r="BB3" s="152"/>
+      <c r="BC3" s="152"/>
+      <c r="BD3" s="152"/>
+      <c r="BE3" s="152"/>
+      <c r="BF3" s="152"/>
+      <c r="BG3" s="153"/>
+      <c r="BH3" s="151"/>
+      <c r="BI3" s="152"/>
+      <c r="BJ3" s="152"/>
+      <c r="BK3" s="152"/>
+      <c r="BL3" s="152"/>
+      <c r="BM3" s="152"/>
+      <c r="BN3" s="153"/>
+    </row>
+    <row r="4" spans="1:150" s="144" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A4" s="146"/>
+      <c r="B4" s="149" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="193">
+      <c r="C4" s="217">
         <v>43507</v>
       </c>
-      <c r="D4" s="194"/>
-      <c r="E4" s="195"/>
-      <c r="H4" s="150" t="s">
+      <c r="D4" s="218"/>
+      <c r="E4" s="219"/>
+      <c r="H4" s="149" t="s">
         <v>74</v>
       </c>
-      <c r="I4" s="151">
+      <c r="I4" s="150">
         <v>1</v>
       </c>
-      <c r="K4" s="191" t="str">
+      <c r="K4" s="215" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="186"/>
-      <c r="M4" s="186"/>
-      <c r="N4" s="186"/>
-      <c r="O4" s="186"/>
-      <c r="P4" s="186"/>
-      <c r="Q4" s="196"/>
-      <c r="R4" s="191" t="str">
+      <c r="L4" s="193"/>
+      <c r="M4" s="193"/>
+      <c r="N4" s="193"/>
+      <c r="O4" s="193"/>
+      <c r="P4" s="193"/>
+      <c r="Q4" s="220"/>
+      <c r="R4" s="215" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="186"/>
-      <c r="T4" s="186"/>
-      <c r="U4" s="186"/>
-      <c r="V4" s="186"/>
-      <c r="W4" s="186"/>
-      <c r="X4" s="192"/>
-      <c r="Y4" s="200" t="str">
+      <c r="S4" s="193"/>
+      <c r="T4" s="193"/>
+      <c r="U4" s="193"/>
+      <c r="V4" s="193"/>
+      <c r="W4" s="193"/>
+      <c r="X4" s="216"/>
+      <c r="Y4" s="224" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="186"/>
-      <c r="AA4" s="186"/>
-      <c r="AB4" s="186"/>
-      <c r="AC4" s="186"/>
-      <c r="AD4" s="186"/>
-      <c r="AE4" s="201"/>
-      <c r="AF4" s="185" t="str">
+      <c r="Z4" s="193"/>
+      <c r="AA4" s="193"/>
+      <c r="AB4" s="193"/>
+      <c r="AC4" s="193"/>
+      <c r="AD4" s="193"/>
+      <c r="AE4" s="225"/>
+      <c r="AF4" s="211" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="186"/>
-      <c r="AH4" s="186"/>
-      <c r="AI4" s="186"/>
-      <c r="AJ4" s="186"/>
-      <c r="AK4" s="186"/>
-      <c r="AL4" s="187"/>
-      <c r="AM4" s="214" t="str">
+      <c r="AG4" s="193"/>
+      <c r="AH4" s="193"/>
+      <c r="AI4" s="193"/>
+      <c r="AJ4" s="193"/>
+      <c r="AK4" s="193"/>
+      <c r="AL4" s="212"/>
+      <c r="AM4" s="204" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="186"/>
-      <c r="AO4" s="186"/>
-      <c r="AP4" s="186"/>
-      <c r="AQ4" s="186"/>
-      <c r="AR4" s="186"/>
-      <c r="AS4" s="215"/>
-      <c r="AT4" s="210" t="str">
+      <c r="AN4" s="193"/>
+      <c r="AO4" s="193"/>
+      <c r="AP4" s="193"/>
+      <c r="AQ4" s="193"/>
+      <c r="AR4" s="193"/>
+      <c r="AS4" s="205"/>
+      <c r="AT4" s="200" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="186"/>
-      <c r="AV4" s="186"/>
-      <c r="AW4" s="186"/>
-      <c r="AX4" s="186"/>
-      <c r="AY4" s="186"/>
-      <c r="AZ4" s="211"/>
-      <c r="BA4" s="216" t="str">
+      <c r="AU4" s="193"/>
+      <c r="AV4" s="193"/>
+      <c r="AW4" s="193"/>
+      <c r="AX4" s="193"/>
+      <c r="AY4" s="193"/>
+      <c r="AZ4" s="201"/>
+      <c r="BA4" s="206" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="186"/>
-      <c r="BC4" s="186"/>
-      <c r="BD4" s="186"/>
-      <c r="BE4" s="186"/>
-      <c r="BF4" s="186"/>
-      <c r="BG4" s="217"/>
-      <c r="BH4" s="204" t="str">
+      <c r="BB4" s="193"/>
+      <c r="BC4" s="193"/>
+      <c r="BD4" s="193"/>
+      <c r="BE4" s="193"/>
+      <c r="BF4" s="193"/>
+      <c r="BG4" s="207"/>
+      <c r="BH4" s="192" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="186"/>
-      <c r="BJ4" s="186"/>
-      <c r="BK4" s="186"/>
-      <c r="BL4" s="186"/>
-      <c r="BM4" s="186"/>
-      <c r="BN4" s="205"/>
-    </row>
-    <row r="5" spans="1:150" s="84" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A5" s="148"/>
-      <c r="B5" s="150" t="s">
+      <c r="BI4" s="193"/>
+      <c r="BJ4" s="193"/>
+      <c r="BK4" s="193"/>
+      <c r="BL4" s="193"/>
+      <c r="BM4" s="193"/>
+      <c r="BN4" s="194"/>
+    </row>
+    <row r="5" spans="1:150" s="83" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A5" s="147"/>
+      <c r="B5" s="149" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="193"/>
-      <c r="D5" s="194"/>
-      <c r="E5" s="195"/>
-      <c r="F5" s="146"/>
-      <c r="G5" s="146"/>
-      <c r="H5" s="146"/>
-      <c r="I5" s="146"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="197">
+      <c r="C5" s="217"/>
+      <c r="D5" s="218"/>
+      <c r="E5" s="219"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="221">
         <f>K6</f>
         <v>43507</v>
       </c>
-      <c r="L5" s="189"/>
-      <c r="M5" s="189"/>
-      <c r="N5" s="189"/>
-      <c r="O5" s="189"/>
-      <c r="P5" s="189"/>
-      <c r="Q5" s="199"/>
-      <c r="R5" s="197">
+      <c r="L5" s="196"/>
+      <c r="M5" s="196"/>
+      <c r="N5" s="196"/>
+      <c r="O5" s="196"/>
+      <c r="P5" s="196"/>
+      <c r="Q5" s="223"/>
+      <c r="R5" s="221">
         <f>R6</f>
         <v>43514</v>
       </c>
-      <c r="S5" s="189"/>
-      <c r="T5" s="189"/>
-      <c r="U5" s="189"/>
-      <c r="V5" s="189"/>
-      <c r="W5" s="189"/>
-      <c r="X5" s="198"/>
-      <c r="Y5" s="202">
+      <c r="S5" s="196"/>
+      <c r="T5" s="196"/>
+      <c r="U5" s="196"/>
+      <c r="V5" s="196"/>
+      <c r="W5" s="196"/>
+      <c r="X5" s="222"/>
+      <c r="Y5" s="226">
         <f>Y6</f>
         <v>43521</v>
       </c>
-      <c r="Z5" s="189"/>
-      <c r="AA5" s="189"/>
-      <c r="AB5" s="189"/>
-      <c r="AC5" s="189"/>
-      <c r="AD5" s="189"/>
-      <c r="AE5" s="203"/>
-      <c r="AF5" s="188">
+      <c r="Z5" s="196"/>
+      <c r="AA5" s="196"/>
+      <c r="AB5" s="196"/>
+      <c r="AC5" s="196"/>
+      <c r="AD5" s="196"/>
+      <c r="AE5" s="227"/>
+      <c r="AF5" s="213">
         <f>AF6</f>
         <v>43528</v>
       </c>
-      <c r="AG5" s="189"/>
-      <c r="AH5" s="189"/>
-      <c r="AI5" s="189"/>
-      <c r="AJ5" s="189"/>
-      <c r="AK5" s="189"/>
-      <c r="AL5" s="190"/>
-      <c r="AM5" s="208">
+      <c r="AG5" s="196"/>
+      <c r="AH5" s="196"/>
+      <c r="AI5" s="196"/>
+      <c r="AJ5" s="196"/>
+      <c r="AK5" s="196"/>
+      <c r="AL5" s="214"/>
+      <c r="AM5" s="198">
         <f>AM6</f>
         <v>43535</v>
       </c>
-      <c r="AN5" s="189"/>
-      <c r="AO5" s="189"/>
-      <c r="AP5" s="189"/>
-      <c r="AQ5" s="189"/>
-      <c r="AR5" s="189"/>
-      <c r="AS5" s="209"/>
-      <c r="AT5" s="212">
+      <c r="AN5" s="196"/>
+      <c r="AO5" s="196"/>
+      <c r="AP5" s="196"/>
+      <c r="AQ5" s="196"/>
+      <c r="AR5" s="196"/>
+      <c r="AS5" s="199"/>
+      <c r="AT5" s="202">
         <f>AT6</f>
         <v>43542</v>
       </c>
-      <c r="AU5" s="189"/>
-      <c r="AV5" s="189"/>
-      <c r="AW5" s="189"/>
-      <c r="AX5" s="189"/>
-      <c r="AY5" s="189"/>
-      <c r="AZ5" s="213"/>
-      <c r="BA5" s="218">
+      <c r="AU5" s="196"/>
+      <c r="AV5" s="196"/>
+      <c r="AW5" s="196"/>
+      <c r="AX5" s="196"/>
+      <c r="AY5" s="196"/>
+      <c r="AZ5" s="203"/>
+      <c r="BA5" s="208">
         <f>BA6</f>
         <v>43549</v>
       </c>
-      <c r="BB5" s="189"/>
-      <c r="BC5" s="189"/>
-      <c r="BD5" s="189"/>
-      <c r="BE5" s="189"/>
-      <c r="BF5" s="189"/>
-      <c r="BG5" s="219"/>
-      <c r="BH5" s="206">
+      <c r="BB5" s="196"/>
+      <c r="BC5" s="196"/>
+      <c r="BD5" s="196"/>
+      <c r="BE5" s="196"/>
+      <c r="BF5" s="196"/>
+      <c r="BG5" s="209"/>
+      <c r="BH5" s="195">
         <f>BH6</f>
         <v>43556</v>
       </c>
-      <c r="BI5" s="189"/>
-      <c r="BJ5" s="189"/>
-      <c r="BK5" s="189"/>
-      <c r="BL5" s="189"/>
-      <c r="BM5" s="189"/>
-      <c r="BN5" s="207"/>
-    </row>
-    <row r="6" spans="1:150" s="82" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A6" s="78"/>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="94">
+      <c r="BI5" s="196"/>
+      <c r="BJ5" s="196"/>
+      <c r="BK5" s="196"/>
+      <c r="BL5" s="196"/>
+      <c r="BM5" s="196"/>
+      <c r="BN5" s="197"/>
+    </row>
+    <row r="6" spans="1:150" s="81" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A6" s="77"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="93">
         <f>C4-WEEKDAY(C4,1)+2+7*(I4-1)</f>
         <v>43507</v>
       </c>
-      <c r="L6" s="81">
+      <c r="L6" s="80">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
         <v>43508</v>
       </c>
-      <c r="M6" s="81">
+      <c r="M6" s="80">
         <f t="shared" si="0"/>
         <v>43509</v>
       </c>
-      <c r="N6" s="81">
+      <c r="N6" s="80">
         <f t="shared" si="0"/>
         <v>43510</v>
       </c>
-      <c r="O6" s="81">
+      <c r="O6" s="80">
         <f t="shared" si="0"/>
         <v>43511</v>
       </c>
-      <c r="P6" s="81">
+      <c r="P6" s="80">
         <f t="shared" si="0"/>
         <v>43512</v>
       </c>
-      <c r="Q6" s="95">
+      <c r="Q6" s="94">
         <f t="shared" si="0"/>
         <v>43513</v>
       </c>
-      <c r="R6" s="94">
+      <c r="R6" s="93">
         <f t="shared" si="0"/>
         <v>43514</v>
       </c>
-      <c r="S6" s="81">
+      <c r="S6" s="80">
         <f t="shared" si="0"/>
         <v>43515</v>
       </c>
-      <c r="T6" s="81">
+      <c r="T6" s="80">
         <f t="shared" si="0"/>
         <v>43516</v>
       </c>
-      <c r="U6" s="81">
+      <c r="U6" s="80">
         <f t="shared" ref="U6" si="1">T6+1</f>
         <v>43517</v>
       </c>
-      <c r="V6" s="81">
+      <c r="V6" s="80">
         <f t="shared" ref="V6" si="2">U6+1</f>
         <v>43518</v>
       </c>
-      <c r="W6" s="81">
+      <c r="W6" s="80">
         <f t="shared" ref="W6" si="3">V6+1</f>
         <v>43519</v>
       </c>
-      <c r="X6" s="96">
+      <c r="X6" s="95">
         <f t="shared" si="0"/>
         <v>43520</v>
       </c>
-      <c r="Y6" s="97">
+      <c r="Y6" s="96">
         <f t="shared" si="0"/>
         <v>43521</v>
       </c>
-      <c r="Z6" s="81">
+      <c r="Z6" s="80">
         <f t="shared" si="0"/>
         <v>43522</v>
       </c>
-      <c r="AA6" s="81">
+      <c r="AA6" s="80">
         <f t="shared" si="0"/>
         <v>43523</v>
       </c>
-      <c r="AB6" s="81">
+      <c r="AB6" s="80">
         <f t="shared" si="0"/>
         <v>43524</v>
       </c>
-      <c r="AC6" s="81">
+      <c r="AC6" s="80">
         <f t="shared" si="0"/>
         <v>43525</v>
       </c>
-      <c r="AD6" s="81">
+      <c r="AD6" s="80">
         <f t="shared" si="0"/>
         <v>43526</v>
       </c>
-      <c r="AE6" s="98">
+      <c r="AE6" s="97">
         <f t="shared" si="0"/>
         <v>43527</v>
       </c>
-      <c r="AF6" s="99">
+      <c r="AF6" s="98">
         <f t="shared" si="0"/>
         <v>43528</v>
       </c>
-      <c r="AG6" s="81">
+      <c r="AG6" s="80">
         <f t="shared" si="0"/>
         <v>43529</v>
       </c>
-      <c r="AH6" s="81">
+      <c r="AH6" s="80">
         <f t="shared" si="0"/>
         <v>43530</v>
       </c>
-      <c r="AI6" s="81">
+      <c r="AI6" s="80">
         <f t="shared" si="0"/>
         <v>43531</v>
       </c>
-      <c r="AJ6" s="81">
+      <c r="AJ6" s="80">
         <f t="shared" si="0"/>
         <v>43532</v>
       </c>
-      <c r="AK6" s="81">
+      <c r="AK6" s="80">
         <f t="shared" si="0"/>
         <v>43533</v>
       </c>
-      <c r="AL6" s="100">
+      <c r="AL6" s="99">
         <f t="shared" si="0"/>
         <v>43534</v>
       </c>
-      <c r="AM6" s="101">
+      <c r="AM6" s="100">
         <f t="shared" si="0"/>
         <v>43535</v>
       </c>
-      <c r="AN6" s="81">
+      <c r="AN6" s="80">
         <f t="shared" si="0"/>
         <v>43536</v>
       </c>
-      <c r="AO6" s="81">
+      <c r="AO6" s="80">
         <f t="shared" si="0"/>
         <v>43537</v>
       </c>
-      <c r="AP6" s="81">
+      <c r="AP6" s="80">
         <f t="shared" si="0"/>
         <v>43538</v>
       </c>
-      <c r="AQ6" s="81">
+      <c r="AQ6" s="80">
         <f t="shared" si="0"/>
         <v>43539</v>
       </c>
-      <c r="AR6" s="81">
+      <c r="AR6" s="80">
         <f t="shared" ref="AR6:BN6" si="4">AQ6+1</f>
         <v>43540</v>
       </c>
-      <c r="AS6" s="102">
+      <c r="AS6" s="101">
         <f t="shared" si="4"/>
         <v>43541</v>
       </c>
-      <c r="AT6" s="103">
+      <c r="AT6" s="102">
         <f t="shared" si="4"/>
         <v>43542</v>
       </c>
-      <c r="AU6" s="81">
+      <c r="AU6" s="80">
         <f t="shared" si="4"/>
         <v>43543</v>
       </c>
-      <c r="AV6" s="81">
+      <c r="AV6" s="80">
         <f t="shared" si="4"/>
         <v>43544</v>
       </c>
-      <c r="AW6" s="81">
+      <c r="AW6" s="80">
         <f t="shared" si="4"/>
         <v>43545</v>
       </c>
-      <c r="AX6" s="81">
+      <c r="AX6" s="80">
         <f t="shared" si="4"/>
         <v>43546</v>
       </c>
-      <c r="AY6" s="81">
+      <c r="AY6" s="80">
         <f t="shared" si="4"/>
         <v>43547</v>
       </c>
-      <c r="AZ6" s="104">
+      <c r="AZ6" s="103">
         <f t="shared" si="4"/>
         <v>43548</v>
       </c>
-      <c r="BA6" s="105">
+      <c r="BA6" s="104">
         <f t="shared" si="4"/>
         <v>43549</v>
       </c>
-      <c r="BB6" s="81">
+      <c r="BB6" s="80">
         <f t="shared" si="4"/>
         <v>43550</v>
       </c>
-      <c r="BC6" s="81">
+      <c r="BC6" s="80">
         <f t="shared" si="4"/>
         <v>43551</v>
       </c>
-      <c r="BD6" s="81">
+      <c r="BD6" s="80">
         <f t="shared" si="4"/>
         <v>43552</v>
       </c>
-      <c r="BE6" s="81">
+      <c r="BE6" s="80">
         <f t="shared" si="4"/>
         <v>43553</v>
       </c>
-      <c r="BF6" s="81">
+      <c r="BF6" s="80">
         <f t="shared" si="4"/>
         <v>43554</v>
       </c>
-      <c r="BG6" s="106">
+      <c r="BG6" s="105">
         <f t="shared" si="4"/>
         <v>43555</v>
       </c>
-      <c r="BH6" s="107">
+      <c r="BH6" s="106">
         <f t="shared" si="4"/>
         <v>43556</v>
       </c>
-      <c r="BI6" s="81">
+      <c r="BI6" s="80">
         <f t="shared" si="4"/>
         <v>43557</v>
       </c>
-      <c r="BJ6" s="81">
+      <c r="BJ6" s="80">
         <f t="shared" si="4"/>
         <v>43558</v>
       </c>
-      <c r="BK6" s="81">
+      <c r="BK6" s="80">
         <f t="shared" si="4"/>
         <v>43559</v>
       </c>
-      <c r="BL6" s="81">
+      <c r="BL6" s="80">
         <f t="shared" si="4"/>
         <v>43560</v>
       </c>
-      <c r="BM6" s="81">
+      <c r="BM6" s="80">
         <f t="shared" si="4"/>
         <v>43561</v>
       </c>
-      <c r="BN6" s="108">
+      <c r="BN6" s="107">
         <f t="shared" si="4"/>
         <v>43562</v>
       </c>
     </row>
-    <row r="7" spans="1:150" s="77" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A7" s="70" t="s">
+    <row r="7" spans="1:150" s="76" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A7" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="73" t="s">
+      <c r="D7" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="74" t="s">
+      <c r="E7" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="74" t="s">
+      <c r="F7" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="72" t="s">
+      <c r="G7" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="H7" s="72" t="s">
+      <c r="H7" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="I7" s="112" t="s">
+      <c r="I7" s="111" t="s">
         <v>72</v>
       </c>
-      <c r="J7" s="69"/>
-      <c r="K7" s="91" t="str">
+      <c r="J7" s="111" t="s">
+        <v>155</v>
+      </c>
+      <c r="K7" s="90" t="str">
         <f t="shared" ref="K7:AP7" si="5">CHOOSE(WEEKDAY(K6,1),"S","M","T","W","T","F","S")</f>
         <v>M</v>
       </c>
-      <c r="L7" s="75" t="str">
+      <c r="L7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="M7" s="75" t="str">
+      <c r="M7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>W</v>
       </c>
-      <c r="N7" s="75" t="str">
+      <c r="N7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="O7" s="75" t="str">
+      <c r="O7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="P7" s="75" t="str">
+      <c r="P7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>S</v>
       </c>
-      <c r="Q7" s="92" t="str">
+      <c r="Q7" s="91" t="str">
         <f t="shared" si="5"/>
         <v>S</v>
       </c>
-      <c r="R7" s="91" t="str">
+      <c r="R7" s="90" t="str">
         <f t="shared" si="5"/>
         <v>M</v>
       </c>
-      <c r="S7" s="75" t="str">
+      <c r="S7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="T7" s="75" t="str">
+      <c r="T7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>W</v>
       </c>
-      <c r="U7" s="75" t="str">
+      <c r="U7" s="74" t="str">
         <f t="shared" ref="U7:W7" si="6">CHOOSE(WEEKDAY(U6,1),"S","M","T","W","T","F","S")</f>
         <v>T</v>
       </c>
-      <c r="V7" s="75" t="str">
+      <c r="V7" s="74" t="str">
         <f t="shared" si="6"/>
         <v>F</v>
       </c>
-      <c r="W7" s="75" t="str">
+      <c r="W7" s="74" t="str">
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="X7" s="92" t="str">
+      <c r="X7" s="91" t="str">
         <f t="shared" si="5"/>
         <v>S</v>
       </c>
-      <c r="Y7" s="90" t="str">
+      <c r="Y7" s="89" t="str">
         <f t="shared" si="5"/>
         <v>M</v>
       </c>
-      <c r="Z7" s="75" t="str">
+      <c r="Z7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="AA7" s="75" t="str">
+      <c r="AA7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>W</v>
       </c>
-      <c r="AB7" s="75" t="str">
+      <c r="AB7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="AC7" s="75" t="str">
+      <c r="AC7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="AD7" s="75" t="str">
+      <c r="AD7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>S</v>
       </c>
-      <c r="AE7" s="93" t="str">
+      <c r="AE7" s="92" t="str">
         <f t="shared" si="5"/>
         <v>S</v>
       </c>
-      <c r="AF7" s="91" t="str">
+      <c r="AF7" s="90" t="str">
         <f t="shared" si="5"/>
         <v>M</v>
       </c>
-      <c r="AG7" s="75" t="str">
+      <c r="AG7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="AH7" s="75" t="str">
+      <c r="AH7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>W</v>
       </c>
-      <c r="AI7" s="75" t="str">
+      <c r="AI7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="AJ7" s="75" t="str">
+      <c r="AJ7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="AK7" s="75" t="str">
+      <c r="AK7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>S</v>
       </c>
-      <c r="AL7" s="92" t="str">
+      <c r="AL7" s="91" t="str">
         <f t="shared" si="5"/>
         <v>S</v>
       </c>
-      <c r="AM7" s="91" t="str">
+      <c r="AM7" s="90" t="str">
         <f t="shared" si="5"/>
         <v>M</v>
       </c>
-      <c r="AN7" s="75" t="str">
+      <c r="AN7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="AO7" s="75" t="str">
+      <c r="AO7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>W</v>
       </c>
-      <c r="AP7" s="75" t="str">
+      <c r="AP7" s="74" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="AQ7" s="75" t="str">
+      <c r="AQ7" s="74" t="str">
         <f t="shared" ref="AQ7:BN7" si="7">CHOOSE(WEEKDAY(AQ6,1),"S","M","T","W","T","F","S")</f>
         <v>F</v>
       </c>
-      <c r="AR7" s="75" t="str">
+      <c r="AR7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>S</v>
       </c>
-      <c r="AS7" s="92" t="str">
+      <c r="AS7" s="91" t="str">
         <f t="shared" si="7"/>
         <v>S</v>
       </c>
-      <c r="AT7" s="91" t="str">
+      <c r="AT7" s="90" t="str">
         <f t="shared" si="7"/>
         <v>M</v>
       </c>
-      <c r="AU7" s="75" t="str">
+      <c r="AU7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>T</v>
       </c>
-      <c r="AV7" s="75" t="str">
+      <c r="AV7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>W</v>
       </c>
-      <c r="AW7" s="75" t="str">
+      <c r="AW7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>T</v>
       </c>
-      <c r="AX7" s="75" t="str">
+      <c r="AX7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>F</v>
       </c>
-      <c r="AY7" s="75" t="str">
+      <c r="AY7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>S</v>
       </c>
-      <c r="AZ7" s="92" t="str">
+      <c r="AZ7" s="91" t="str">
         <f t="shared" si="7"/>
         <v>S</v>
       </c>
-      <c r="BA7" s="91" t="str">
+      <c r="BA7" s="90" t="str">
         <f t="shared" si="7"/>
         <v>M</v>
       </c>
-      <c r="BB7" s="75" t="str">
+      <c r="BB7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>T</v>
       </c>
-      <c r="BC7" s="75" t="str">
+      <c r="BC7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>W</v>
       </c>
-      <c r="BD7" s="75" t="str">
+      <c r="BD7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>T</v>
       </c>
-      <c r="BE7" s="75" t="str">
+      <c r="BE7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>F</v>
       </c>
-      <c r="BF7" s="75" t="str">
+      <c r="BF7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>S</v>
       </c>
-      <c r="BG7" s="92" t="str">
+      <c r="BG7" s="91" t="str">
         <f t="shared" si="7"/>
         <v>S</v>
       </c>
-      <c r="BH7" s="91" t="str">
+      <c r="BH7" s="90" t="str">
         <f t="shared" si="7"/>
         <v>M</v>
       </c>
-      <c r="BI7" s="75" t="str">
+      <c r="BI7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>T</v>
       </c>
-      <c r="BJ7" s="75" t="str">
+      <c r="BJ7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>W</v>
       </c>
-      <c r="BK7" s="75" t="str">
+      <c r="BK7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>T</v>
       </c>
-      <c r="BL7" s="75" t="str">
+      <c r="BL7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>F</v>
       </c>
-      <c r="BM7" s="75" t="str">
+      <c r="BM7" s="74" t="str">
         <f t="shared" si="7"/>
         <v>S</v>
       </c>
-      <c r="BN7" s="92" t="str">
+      <c r="BN7" s="91" t="str">
         <f t="shared" si="7"/>
         <v>S</v>
       </c>
-      <c r="BO7" s="76"/>
-      <c r="BP7" s="76"/>
-      <c r="BQ7" s="76"/>
-      <c r="BR7" s="76"/>
-      <c r="BS7" s="76"/>
-      <c r="BT7" s="76"/>
-      <c r="BU7" s="76"/>
-      <c r="BV7" s="76"/>
-      <c r="BW7" s="76"/>
-      <c r="BX7" s="76"/>
-      <c r="BY7" s="76"/>
-      <c r="BZ7" s="76"/>
-      <c r="CA7" s="76"/>
-      <c r="CB7" s="76"/>
-      <c r="CC7" s="76"/>
-      <c r="CD7" s="76"/>
-      <c r="CE7" s="76"/>
-      <c r="CF7" s="76"/>
-      <c r="CG7" s="76"/>
-      <c r="CH7" s="76"/>
-      <c r="CI7" s="76"/>
-      <c r="CJ7" s="76"/>
-      <c r="CK7" s="76"/>
-      <c r="CL7" s="76"/>
-      <c r="CM7" s="76"/>
-      <c r="CN7" s="76"/>
-      <c r="CO7" s="76"/>
-      <c r="CP7" s="76"/>
-      <c r="CQ7" s="76"/>
-      <c r="CR7" s="76"/>
-      <c r="CS7" s="76"/>
-      <c r="CT7" s="76"/>
-      <c r="CU7" s="76"/>
-      <c r="CV7" s="76"/>
-      <c r="CW7" s="76"/>
-      <c r="CX7" s="76"/>
-      <c r="CY7" s="76"/>
-      <c r="CZ7" s="76"/>
-      <c r="DA7" s="76"/>
-      <c r="DB7" s="76"/>
-      <c r="DC7" s="76"/>
-      <c r="DD7" s="76"/>
-      <c r="DE7" s="76"/>
-      <c r="DF7" s="76"/>
-      <c r="DG7" s="76"/>
-      <c r="DH7" s="76"/>
-      <c r="DI7" s="76"/>
-      <c r="DJ7" s="76"/>
-      <c r="DK7" s="76"/>
-      <c r="DL7" s="76"/>
-      <c r="DM7" s="76"/>
-      <c r="DN7" s="76"/>
-      <c r="DO7" s="76"/>
-      <c r="DP7" s="76"/>
-      <c r="DQ7" s="76"/>
-      <c r="DR7" s="76"/>
-      <c r="DS7" s="76"/>
-      <c r="DT7" s="76"/>
-      <c r="DU7" s="76"/>
-      <c r="DV7" s="76"/>
-      <c r="DW7" s="76"/>
-      <c r="DX7" s="76"/>
-      <c r="DY7" s="76"/>
-      <c r="DZ7" s="76"/>
-      <c r="EA7" s="76"/>
-      <c r="EB7" s="76"/>
-      <c r="EC7" s="76"/>
-      <c r="ED7" s="76"/>
-      <c r="EE7" s="76"/>
-      <c r="EF7" s="76"/>
-      <c r="EG7" s="76"/>
-      <c r="EH7" s="76"/>
-      <c r="EI7" s="76"/>
-      <c r="EJ7" s="76"/>
-      <c r="EK7" s="76"/>
-      <c r="EL7" s="76"/>
-      <c r="EM7" s="76"/>
-      <c r="EN7" s="76"/>
-      <c r="EO7" s="76"/>
-      <c r="EP7" s="76"/>
-      <c r="EQ7" s="76"/>
-      <c r="ER7" s="76"/>
-      <c r="ES7" s="76"/>
-      <c r="ET7" s="76"/>
+      <c r="BO7" s="75"/>
+      <c r="BP7" s="75"/>
+      <c r="BQ7" s="75"/>
+      <c r="BR7" s="75"/>
+      <c r="BS7" s="75"/>
+      <c r="BT7" s="75"/>
+      <c r="BU7" s="75"/>
+      <c r="BV7" s="75"/>
+      <c r="BW7" s="75"/>
+      <c r="BX7" s="75"/>
+      <c r="BY7" s="75"/>
+      <c r="BZ7" s="75"/>
+      <c r="CA7" s="75"/>
+      <c r="CB7" s="75"/>
+      <c r="CC7" s="75"/>
+      <c r="CD7" s="75"/>
+      <c r="CE7" s="75"/>
+      <c r="CF7" s="75"/>
+      <c r="CG7" s="75"/>
+      <c r="CH7" s="75"/>
+      <c r="CI7" s="75"/>
+      <c r="CJ7" s="75"/>
+      <c r="CK7" s="75"/>
+      <c r="CL7" s="75"/>
+      <c r="CM7" s="75"/>
+      <c r="CN7" s="75"/>
+      <c r="CO7" s="75"/>
+      <c r="CP7" s="75"/>
+      <c r="CQ7" s="75"/>
+      <c r="CR7" s="75"/>
+      <c r="CS7" s="75"/>
+      <c r="CT7" s="75"/>
+      <c r="CU7" s="75"/>
+      <c r="CV7" s="75"/>
+      <c r="CW7" s="75"/>
+      <c r="CX7" s="75"/>
+      <c r="CY7" s="75"/>
+      <c r="CZ7" s="75"/>
+      <c r="DA7" s="75"/>
+      <c r="DB7" s="75"/>
+      <c r="DC7" s="75"/>
+      <c r="DD7" s="75"/>
+      <c r="DE7" s="75"/>
+      <c r="DF7" s="75"/>
+      <c r="DG7" s="75"/>
+      <c r="DH7" s="75"/>
+      <c r="DI7" s="75"/>
+      <c r="DJ7" s="75"/>
+      <c r="DK7" s="75"/>
+      <c r="DL7" s="75"/>
+      <c r="DM7" s="75"/>
+      <c r="DN7" s="75"/>
+      <c r="DO7" s="75"/>
+      <c r="DP7" s="75"/>
+      <c r="DQ7" s="75"/>
+      <c r="DR7" s="75"/>
+      <c r="DS7" s="75"/>
+      <c r="DT7" s="75"/>
+      <c r="DU7" s="75"/>
+      <c r="DV7" s="75"/>
+      <c r="DW7" s="75"/>
+      <c r="DX7" s="75"/>
+      <c r="DY7" s="75"/>
+      <c r="DZ7" s="75"/>
+      <c r="EA7" s="75"/>
+      <c r="EB7" s="75"/>
+      <c r="EC7" s="75"/>
+      <c r="ED7" s="75"/>
+      <c r="EE7" s="75"/>
+      <c r="EF7" s="75"/>
+      <c r="EG7" s="75"/>
+      <c r="EH7" s="75"/>
+      <c r="EI7" s="75"/>
+      <c r="EJ7" s="75"/>
+      <c r="EK7" s="75"/>
+      <c r="EL7" s="75"/>
+      <c r="EM7" s="75"/>
+      <c r="EN7" s="75"/>
+      <c r="EO7" s="75"/>
+      <c r="EP7" s="75"/>
+      <c r="EQ7" s="75"/>
+      <c r="ER7" s="75"/>
+      <c r="ES7" s="75"/>
+      <c r="ET7" s="75"/>
     </row>
     <row r="8" spans="1:150" s="37" customFormat="1" ht="19" thickTop="1">
-      <c r="A8" s="121" t="str">
+      <c r="A8" s="120" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
       </c>
-      <c r="B8" s="109" t="s">
+      <c r="B8" s="108" t="s">
         <v>134</v>
       </c>
       <c r="D8" s="38"/>
@@ -5347,8 +5503,8 @@
       <c r="F8" s="39"/>
       <c r="G8" s="40"/>
       <c r="H8" s="41"/>
-      <c r="I8" s="137"/>
-      <c r="J8" s="124"/>
+      <c r="I8" s="136"/>
+      <c r="J8" s="123"/>
       <c r="K8" s="42"/>
       <c r="L8" s="42"/>
       <c r="M8" s="42"/>
@@ -5407,19 +5563,19 @@
       <c r="BN8" s="42"/>
     </row>
     <row r="9" spans="1:150" s="45" customFormat="1" ht="18">
-      <c r="A9" s="122" t="str">
+      <c r="A9" s="121" t="str">
         <f t="shared" ref="A9:A15" si="8">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
-      <c r="B9" s="118" t="s">
+      <c r="B9" s="117" t="s">
         <v>135</v>
       </c>
-      <c r="C9" s="119" t="s">
+      <c r="C9" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="D9" s="120"/>
-      <c r="E9" s="117"/>
-      <c r="F9" s="113" t="str">
+      <c r="D9" s="119"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="112" t="str">
         <f>IF(ISBLANK(E9)," - ",IF(G9=0,E9,E9+G9-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
@@ -5429,11 +5585,11 @@
       <c r="H9" s="68">
         <v>0</v>
       </c>
-      <c r="I9" s="135">
+      <c r="I9" s="134">
         <f>IF(OR(F9=0,E9=0),0,NETWORKDAYS(E9,F9))</f>
         <v>0</v>
       </c>
-      <c r="J9" s="125"/>
+      <c r="J9" s="239"/>
       <c r="K9" s="47"/>
       <c r="L9" s="47"/>
       <c r="M9" s="47"/>
@@ -5492,19 +5648,19 @@
       <c r="BN9" s="47"/>
     </row>
     <row r="10" spans="1:150" s="45" customFormat="1" ht="18">
-      <c r="A10" s="122" t="str">
+      <c r="A10" s="121" t="str">
         <f t="shared" si="8"/>
         <v>1.2</v>
       </c>
-      <c r="B10" s="118" t="s">
+      <c r="B10" s="117" t="s">
         <v>136</v>
       </c>
-      <c r="C10" s="119" t="s">
+      <c r="C10" s="118" t="s">
         <v>138</v>
       </c>
-      <c r="D10" s="120"/>
-      <c r="E10" s="117"/>
-      <c r="F10" s="113" t="str">
+      <c r="D10" s="119"/>
+      <c r="E10" s="116"/>
+      <c r="F10" s="112" t="str">
         <f>IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
@@ -5514,12 +5670,12 @@
       <c r="H10" s="68">
         <v>0</v>
       </c>
-      <c r="I10" s="135">
-        <f t="shared" ref="I9:I18" si="9">IF(OR(F10=0,E10=0),0,NETWORKDAYS(E10,F10))</f>
+      <c r="I10" s="134">
+        <f t="shared" ref="I10:I18" si="9">IF(OR(F10=0,E10=0),0,NETWORKDAYS(E10,F10))</f>
         <v>0</v>
       </c>
-      <c r="J10" s="125"/>
-      <c r="K10" s="47"/>
+      <c r="J10" s="229"/>
+      <c r="K10" s="240"/>
       <c r="L10" s="47"/>
       <c r="M10" s="47"/>
       <c r="N10" s="47"/>
@@ -5577,20 +5733,20 @@
       <c r="BN10" s="47"/>
     </row>
     <row r="11" spans="1:150" s="45" customFormat="1" ht="18">
-      <c r="A11" s="122" t="str">
+      <c r="A11" s="121" t="str">
         <f t="shared" si="8"/>
         <v>1.3</v>
       </c>
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="117" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="119" t="s">
+      <c r="C11" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="D11" s="120"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="113" t="str">
-        <f t="shared" ref="F9:F15" si="10">IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
+      <c r="D11" s="119"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="112" t="str">
+        <f t="shared" ref="F11:F14" si="10">IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G11" s="67">
@@ -5599,12 +5755,12 @@
       <c r="H11" s="68">
         <v>0</v>
       </c>
-      <c r="I11" s="135">
+      <c r="I11" s="134">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J11" s="125"/>
-      <c r="K11" s="47"/>
+      <c r="J11" s="229"/>
+      <c r="K11" s="240"/>
       <c r="L11" s="47"/>
       <c r="M11" s="47"/>
       <c r="N11" s="47"/>
@@ -5662,19 +5818,19 @@
       <c r="BN11" s="47"/>
     </row>
     <row r="12" spans="1:150" s="45" customFormat="1" ht="18">
-      <c r="A12" s="122" t="str">
+      <c r="A12" s="121" t="str">
         <f t="shared" si="8"/>
         <v>1.4</v>
       </c>
-      <c r="B12" s="118" t="s">
+      <c r="B12" s="117" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="C12" s="118" t="s">
         <v>142</v>
       </c>
-      <c r="D12" s="120"/>
-      <c r="E12" s="117"/>
-      <c r="F12" s="113" t="str">
+      <c r="D12" s="119"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="112" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> - </v>
       </c>
@@ -5684,12 +5840,12 @@
       <c r="H12" s="68">
         <v>0</v>
       </c>
-      <c r="I12" s="135">
+      <c r="I12" s="134">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J12" s="125"/>
-      <c r="K12" s="47"/>
+      <c r="J12" s="229"/>
+      <c r="K12" s="240"/>
       <c r="L12" s="47"/>
       <c r="M12" s="47"/>
       <c r="N12" s="47"/>
@@ -5747,19 +5903,19 @@
       <c r="BN12" s="47"/>
     </row>
     <row r="13" spans="1:150" s="45" customFormat="1" ht="26">
-      <c r="A13" s="122" t="str">
+      <c r="A13" s="121" t="str">
         <f t="shared" si="8"/>
         <v>1.5</v>
       </c>
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="117" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="119" t="s">
+      <c r="C13" s="118" t="s">
         <v>143</v>
       </c>
-      <c r="D13" s="120"/>
-      <c r="E13" s="117"/>
-      <c r="F13" s="113" t="str">
+      <c r="D13" s="119"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="112" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> - </v>
       </c>
@@ -5769,12 +5925,12 @@
       <c r="H13" s="68">
         <v>0</v>
       </c>
-      <c r="I13" s="135">
+      <c r="I13" s="134">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J13" s="125"/>
-      <c r="K13" s="47"/>
+      <c r="J13" s="229"/>
+      <c r="K13" s="240"/>
       <c r="L13" s="47"/>
       <c r="M13" s="47"/>
       <c r="N13" s="47"/>
@@ -5832,19 +5988,19 @@
       <c r="BN13" s="47"/>
     </row>
     <row r="14" spans="1:150" s="45" customFormat="1" ht="26">
-      <c r="A14" s="122" t="str">
+      <c r="A14" s="121" t="str">
         <f t="shared" si="8"/>
         <v>1.6</v>
       </c>
-      <c r="B14" s="118" t="s">
+      <c r="B14" s="117" t="s">
         <v>144</v>
       </c>
-      <c r="C14" s="119" t="s">
+      <c r="C14" s="118" t="s">
         <v>143</v>
       </c>
-      <c r="D14" s="120"/>
-      <c r="E14" s="117"/>
-      <c r="F14" s="113" t="str">
+      <c r="D14" s="119"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="112" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> - </v>
       </c>
@@ -5854,11 +6010,11 @@
       <c r="H14" s="68">
         <v>0</v>
       </c>
-      <c r="I14" s="135">
+      <c r="I14" s="134">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J14" s="125"/>
+      <c r="J14" s="241"/>
       <c r="K14" s="47"/>
       <c r="L14" s="47"/>
       <c r="M14" s="47"/>
@@ -5917,19 +6073,19 @@
       <c r="BN14" s="47"/>
     </row>
     <row r="15" spans="1:150" s="45" customFormat="1" ht="18">
-      <c r="A15" s="122" t="str">
+      <c r="A15" s="121" t="str">
         <f t="shared" si="8"/>
         <v>1.7</v>
       </c>
-      <c r="B15" s="118" t="s">
+      <c r="B15" s="117" t="s">
         <v>145</v>
       </c>
-      <c r="C15" s="119" t="s">
+      <c r="C15" s="118" t="s">
         <v>146</v>
       </c>
-      <c r="D15" s="120"/>
-      <c r="E15" s="117"/>
-      <c r="F15" s="113" t="str">
+      <c r="D15" s="119"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="112" t="str">
         <f>IF(ISBLANK(E15)," - ",IF(G15=0,E15,E15+G15-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
@@ -5939,12 +6095,12 @@
       <c r="H15" s="68">
         <v>0</v>
       </c>
-      <c r="I15" s="135">
+      <c r="I15" s="134">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J15" s="125"/>
-      <c r="K15" s="47"/>
+      <c r="J15" s="229"/>
+      <c r="K15" s="240"/>
       <c r="L15" s="47"/>
       <c r="M15" s="47"/>
       <c r="N15" s="47"/>
@@ -6002,33 +6158,33 @@
       <c r="BN15" s="47"/>
     </row>
     <row r="16" spans="1:150" s="45" customFormat="1" ht="18">
-      <c r="A16" s="122" t="s">
+      <c r="A16" s="121" t="s">
         <v>147</v>
       </c>
-      <c r="B16" s="228" t="s">
+      <c r="B16" s="188" t="s">
         <v>152</v>
       </c>
-      <c r="C16" s="119" t="s">
+      <c r="C16" s="232" t="s">
         <v>146</v>
       </c>
-      <c r="D16" s="221"/>
-      <c r="E16" s="229"/>
-      <c r="F16" s="223" t="str">
+      <c r="D16" s="183"/>
+      <c r="E16" s="246"/>
+      <c r="F16" s="184" t="str">
         <f>IF(ISBLANK(E16)," - ",IF(G16=0,E16,E16+G16-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G16" s="224">
+      <c r="G16" s="185">
         <v>0</v>
       </c>
-      <c r="H16" s="225">
+      <c r="H16" s="186">
         <v>0</v>
       </c>
-      <c r="I16" s="226">
+      <c r="I16" s="187">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J16" s="227"/>
-      <c r="K16" s="47"/>
+      <c r="J16" s="242"/>
+      <c r="K16" s="240"/>
       <c r="L16" s="47"/>
       <c r="M16" s="47"/>
       <c r="N16" s="47"/>
@@ -6086,33 +6242,33 @@
       <c r="BN16" s="47"/>
     </row>
     <row r="17" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A17" s="122" t="s">
+      <c r="A17" s="121" t="s">
         <v>148</v>
       </c>
-      <c r="B17" s="228" t="s">
+      <c r="B17" s="234" t="s">
         <v>151</v>
       </c>
-      <c r="C17" s="119" t="s">
+      <c r="C17" s="233" t="s">
         <v>138</v>
       </c>
-      <c r="D17" s="221"/>
-      <c r="E17" s="222"/>
-      <c r="F17" s="223" t="str">
+      <c r="D17" s="183"/>
+      <c r="E17" s="231"/>
+      <c r="F17" s="184" t="str">
         <f>IF(ISBLANK(E17)," - ",IF(G17=0,E17,E17+G17-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G17" s="230">
+      <c r="G17" s="189">
         <v>0</v>
       </c>
-      <c r="H17" s="231">
+      <c r="H17" s="190">
         <v>0</v>
       </c>
-      <c r="I17" s="226">
+      <c r="I17" s="187">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J17" s="227"/>
-      <c r="K17" s="47"/>
+      <c r="J17" s="243"/>
+      <c r="K17" s="240"/>
       <c r="L17" s="47"/>
       <c r="M17" s="47"/>
       <c r="N17" s="47"/>
@@ -6170,33 +6326,33 @@
       <c r="BN17" s="47"/>
     </row>
     <row r="18" spans="1:66" s="45" customFormat="1" ht="26">
-      <c r="A18" s="122" t="s">
+      <c r="A18" s="121" t="s">
         <v>149</v>
       </c>
-      <c r="B18" s="118" t="s">
+      <c r="B18" s="236" t="s">
         <v>150</v>
       </c>
-      <c r="C18" s="235" t="s">
+      <c r="C18" s="233" t="s">
         <v>142</v>
       </c>
-      <c r="D18" s="221"/>
-      <c r="E18" s="234"/>
-      <c r="F18" s="223" t="str">
+      <c r="D18" s="183"/>
+      <c r="E18" s="235"/>
+      <c r="F18" s="184" t="str">
         <f>IF(ISBLANK(E18)," - ",IF(G18=0,E18,E18+G18-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G18" s="230">
+      <c r="G18" s="237">
         <v>0</v>
       </c>
-      <c r="H18" s="231">
+      <c r="H18" s="238">
         <v>0</v>
       </c>
-      <c r="I18" s="226">
+      <c r="I18" s="187">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J18" s="227"/>
-      <c r="K18" s="47"/>
+      <c r="J18" s="230"/>
+      <c r="K18" s="240"/>
       <c r="L18" s="47"/>
       <c r="M18" s="47"/>
       <c r="N18" s="47"/>
@@ -6254,21 +6410,21 @@
       <c r="BN18" s="47"/>
     </row>
     <row r="19" spans="1:66" s="43" customFormat="1" ht="18">
-      <c r="A19" s="123" t="str">
+      <c r="A19" s="122" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
       </c>
-      <c r="B19" s="110" t="s">
+      <c r="B19" s="108" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="37"/>
       <c r="D19" s="49"/>
-      <c r="E19" s="233"/>
-      <c r="F19" s="111"/>
+      <c r="E19" s="191"/>
+      <c r="F19" s="110"/>
       <c r="G19" s="40"/>
-      <c r="H19" s="232"/>
-      <c r="I19" s="136"/>
-      <c r="J19" s="126"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="135"/>
+      <c r="J19" s="125"/>
       <c r="K19" s="52"/>
       <c r="L19" s="52"/>
       <c r="M19" s="52"/>
@@ -6327,7 +6483,7 @@
       <c r="BN19" s="52"/>
     </row>
     <row r="20" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A20" s="122" t="str">
+      <c r="A20" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
       </c>
@@ -6335,10 +6491,10 @@
         <v>7</v>
       </c>
       <c r="D20" s="46"/>
-      <c r="E20" s="117">
+      <c r="E20" s="116">
         <v>43141</v>
       </c>
-      <c r="F20" s="113">
+      <c r="F20" s="112">
         <f t="shared" ref="F20:F24" si="11">IF(ISBLANK(E20)," - ",IF(G20=0,E20,E20+G20-1))</f>
         <v>43144</v>
       </c>
@@ -6348,11 +6504,11 @@
       <c r="H20" s="68">
         <v>0</v>
       </c>
-      <c r="I20" s="135">
+      <c r="I20" s="134">
         <f>IF(OR(F20=0,E20=0),0,NETWORKDAYS(E20,F20))</f>
         <v>2</v>
       </c>
-      <c r="J20" s="125"/>
+      <c r="J20" s="239"/>
       <c r="K20" s="47"/>
       <c r="L20" s="47"/>
       <c r="M20" s="47"/>
@@ -6411,7 +6567,7 @@
       <c r="BN20" s="47"/>
     </row>
     <row r="21" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A21" s="122" t="str">
+      <c r="A21" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.2</v>
       </c>
@@ -6419,10 +6575,10 @@
         <v>7</v>
       </c>
       <c r="D21" s="46"/>
-      <c r="E21" s="117">
+      <c r="E21" s="116">
         <v>43145</v>
       </c>
-      <c r="F21" s="113">
+      <c r="F21" s="112">
         <f t="shared" si="11"/>
         <v>43147</v>
       </c>
@@ -6432,12 +6588,12 @@
       <c r="H21" s="68">
         <v>0</v>
       </c>
-      <c r="I21" s="135">
+      <c r="I21" s="134">
         <f>IF(OR(F21=0,E21=0),0,NETWORKDAYS(E21,F21))</f>
         <v>3</v>
       </c>
-      <c r="J21" s="125"/>
-      <c r="K21" s="47"/>
+      <c r="J21" s="229"/>
+      <c r="K21" s="240"/>
       <c r="L21" s="47"/>
       <c r="M21" s="47"/>
       <c r="N21" s="47"/>
@@ -6495,7 +6651,7 @@
       <c r="BN21" s="47"/>
     </row>
     <row r="22" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A22" s="122" t="str">
+      <c r="A22" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.3</v>
       </c>
@@ -6503,10 +6659,10 @@
         <v>7</v>
       </c>
       <c r="D22" s="46"/>
-      <c r="E22" s="117">
+      <c r="E22" s="116">
         <v>43145</v>
       </c>
-      <c r="F22" s="113">
+      <c r="F22" s="112">
         <f t="shared" si="11"/>
         <v>43147</v>
       </c>
@@ -6516,12 +6672,12 @@
       <c r="H22" s="68">
         <v>0</v>
       </c>
-      <c r="I22" s="135">
+      <c r="I22" s="134">
         <f>IF(OR(F22=0,E22=0),0,NETWORKDAYS(E22,F22))</f>
         <v>3</v>
       </c>
-      <c r="J22" s="125"/>
-      <c r="K22" s="47"/>
+      <c r="J22" s="229"/>
+      <c r="K22" s="240"/>
       <c r="L22" s="47"/>
       <c r="M22" s="47"/>
       <c r="N22" s="47"/>
@@ -6579,7 +6735,7 @@
       <c r="BN22" s="47"/>
     </row>
     <row r="23" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A23" s="122" t="str">
+      <c r="A23" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.4</v>
       </c>
@@ -6587,10 +6743,10 @@
         <v>7</v>
       </c>
       <c r="D23" s="46"/>
-      <c r="E23" s="117">
+      <c r="E23" s="116">
         <v>43148</v>
       </c>
-      <c r="F23" s="113">
+      <c r="F23" s="112">
         <f t="shared" si="11"/>
         <v>43153</v>
       </c>
@@ -6600,12 +6756,12 @@
       <c r="H23" s="68">
         <v>0</v>
       </c>
-      <c r="I23" s="135">
+      <c r="I23" s="134">
         <f>IF(OR(F23=0,E23=0),0,NETWORKDAYS(E23,F23))</f>
         <v>4</v>
       </c>
-      <c r="J23" s="125"/>
-      <c r="K23" s="47"/>
+      <c r="J23" s="229"/>
+      <c r="K23" s="240"/>
       <c r="L23" s="47"/>
       <c r="M23" s="47"/>
       <c r="N23" s="47"/>
@@ -6663,7 +6819,7 @@
       <c r="BN23" s="47"/>
     </row>
     <row r="24" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A24" s="122" t="str">
+      <c r="A24" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.5</v>
       </c>
@@ -6671,10 +6827,10 @@
         <v>7</v>
       </c>
       <c r="D24" s="46"/>
-      <c r="E24" s="117">
+      <c r="E24" s="116">
         <v>43154</v>
       </c>
-      <c r="F24" s="113">
+      <c r="F24" s="112">
         <f t="shared" si="11"/>
         <v>43156</v>
       </c>
@@ -6684,12 +6840,12 @@
       <c r="H24" s="68">
         <v>0</v>
       </c>
-      <c r="I24" s="135">
+      <c r="I24" s="134">
         <f>IF(OR(F24=0,E24=0),0,NETWORKDAYS(E24,F24))</f>
         <v>1</v>
       </c>
-      <c r="J24" s="125"/>
-      <c r="K24" s="47"/>
+      <c r="J24" s="229"/>
+      <c r="K24" s="240"/>
       <c r="L24" s="47"/>
       <c r="M24" s="47"/>
       <c r="N24" s="47"/>
@@ -6747,20 +6903,20 @@
       <c r="BN24" s="47"/>
     </row>
     <row r="25" spans="1:66" s="43" customFormat="1" ht="18">
-      <c r="A25" s="123" t="str">
+      <c r="A25" s="122" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>3</v>
       </c>
-      <c r="B25" s="110" t="s">
+      <c r="B25" s="109" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="49"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="115"/>
+      <c r="E25" s="113"/>
+      <c r="F25" s="114"/>
       <c r="G25" s="50"/>
       <c r="H25" s="51"/>
-      <c r="I25" s="136"/>
-      <c r="J25" s="126"/>
+      <c r="I25" s="135"/>
+      <c r="J25" s="125"/>
       <c r="K25" s="52"/>
       <c r="L25" s="52"/>
       <c r="M25" s="52"/>
@@ -6819,7 +6975,7 @@
       <c r="BN25" s="52"/>
     </row>
     <row r="26" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A26" s="122" t="str">
+      <c r="A26" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
       </c>
@@ -6827,10 +6983,10 @@
         <v>7</v>
       </c>
       <c r="D26" s="46"/>
-      <c r="E26" s="117">
+      <c r="E26" s="116">
         <v>43141</v>
       </c>
-      <c r="F26" s="113">
+      <c r="F26" s="112">
         <f t="shared" ref="F26:F30" si="12">IF(ISBLANK(E26)," - ",IF(G26=0,E26,E26+G26-1))</f>
         <v>43144</v>
       </c>
@@ -6840,12 +6996,12 @@
       <c r="H26" s="68">
         <v>0</v>
       </c>
-      <c r="I26" s="135">
+      <c r="I26" s="134">
         <f>IF(OR(F26=0,E26=0),0,NETWORKDAYS(E26,F26))</f>
         <v>2</v>
       </c>
-      <c r="J26" s="125"/>
-      <c r="K26" s="47"/>
+      <c r="J26" s="229"/>
+      <c r="K26" s="240"/>
       <c r="L26" s="47"/>
       <c r="M26" s="47"/>
       <c r="N26" s="47"/>
@@ -6903,7 +7059,7 @@
       <c r="BN26" s="47"/>
     </row>
     <row r="27" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A27" s="122" t="str">
+      <c r="A27" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.2</v>
       </c>
@@ -6911,10 +7067,10 @@
         <v>7</v>
       </c>
       <c r="D27" s="46"/>
-      <c r="E27" s="117">
+      <c r="E27" s="116">
         <v>43145</v>
       </c>
-      <c r="F27" s="113">
+      <c r="F27" s="112">
         <f t="shared" si="12"/>
         <v>43147</v>
       </c>
@@ -6924,11 +7080,11 @@
       <c r="H27" s="68">
         <v>0</v>
       </c>
-      <c r="I27" s="135">
+      <c r="I27" s="134">
         <f>IF(OR(F27=0,E27=0),0,NETWORKDAYS(E27,F27))</f>
         <v>3</v>
       </c>
-      <c r="J27" s="125"/>
+      <c r="J27" s="241"/>
       <c r="K27" s="47"/>
       <c r="L27" s="47"/>
       <c r="M27" s="47"/>
@@ -6987,7 +7143,7 @@
       <c r="BN27" s="47"/>
     </row>
     <row r="28" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A28" s="122" t="str">
+      <c r="A28" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.3</v>
       </c>
@@ -6995,10 +7151,10 @@
         <v>7</v>
       </c>
       <c r="D28" s="46"/>
-      <c r="E28" s="117">
+      <c r="E28" s="116">
         <v>43145</v>
       </c>
-      <c r="F28" s="113">
+      <c r="F28" s="112">
         <f t="shared" si="12"/>
         <v>43147</v>
       </c>
@@ -7008,11 +7164,11 @@
       <c r="H28" s="68">
         <v>0</v>
       </c>
-      <c r="I28" s="135">
+      <c r="I28" s="134">
         <f>IF(OR(F28=0,E28=0),0,NETWORKDAYS(E28,F28))</f>
         <v>3</v>
       </c>
-      <c r="J28" s="125"/>
+      <c r="J28" s="241"/>
       <c r="K28" s="47"/>
       <c r="L28" s="47"/>
       <c r="M28" s="47"/>
@@ -7071,7 +7227,7 @@
       <c r="BN28" s="47"/>
     </row>
     <row r="29" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A29" s="122" t="str">
+      <c r="A29" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.4</v>
       </c>
@@ -7079,10 +7235,10 @@
         <v>7</v>
       </c>
       <c r="D29" s="46"/>
-      <c r="E29" s="117">
+      <c r="E29" s="116">
         <v>43148</v>
       </c>
-      <c r="F29" s="113">
+      <c r="F29" s="112">
         <f t="shared" si="12"/>
         <v>43153</v>
       </c>
@@ -7092,11 +7248,11 @@
       <c r="H29" s="68">
         <v>0</v>
       </c>
-      <c r="I29" s="135">
+      <c r="I29" s="134">
         <f>IF(OR(F29=0,E29=0),0,NETWORKDAYS(E29,F29))</f>
         <v>4</v>
       </c>
-      <c r="J29" s="125"/>
+      <c r="J29" s="241"/>
       <c r="K29" s="47"/>
       <c r="L29" s="47"/>
       <c r="M29" s="47"/>
@@ -7155,7 +7311,7 @@
       <c r="BN29" s="47"/>
     </row>
     <row r="30" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A30" s="122" t="str">
+      <c r="A30" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.5</v>
       </c>
@@ -7163,10 +7319,10 @@
         <v>7</v>
       </c>
       <c r="D30" s="46"/>
-      <c r="E30" s="117">
+      <c r="E30" s="116">
         <v>43154</v>
       </c>
-      <c r="F30" s="113">
+      <c r="F30" s="112">
         <f t="shared" si="12"/>
         <v>43156</v>
       </c>
@@ -7176,11 +7332,11 @@
       <c r="H30" s="68">
         <v>0</v>
       </c>
-      <c r="I30" s="135">
+      <c r="I30" s="134">
         <f>IF(OR(F30=0,E30=0),0,NETWORKDAYS(E30,F30))</f>
         <v>1</v>
       </c>
-      <c r="J30" s="125"/>
+      <c r="J30" s="244"/>
       <c r="K30" s="47"/>
       <c r="L30" s="47"/>
       <c r="M30" s="47"/>
@@ -7239,20 +7395,20 @@
       <c r="BN30" s="47"/>
     </row>
     <row r="31" spans="1:66" s="43" customFormat="1" ht="18">
-      <c r="A31" s="123" t="str">
+      <c r="A31" s="122" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>4</v>
       </c>
-      <c r="B31" s="110" t="s">
+      <c r="B31" s="109" t="s">
         <v>6</v>
       </c>
       <c r="D31" s="49"/>
-      <c r="E31" s="114"/>
-      <c r="F31" s="115"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="114"/>
       <c r="G31" s="50"/>
       <c r="H31" s="51"/>
-      <c r="I31" s="136"/>
-      <c r="J31" s="126"/>
+      <c r="I31" s="135"/>
+      <c r="J31" s="245"/>
       <c r="K31" s="52"/>
       <c r="L31" s="52"/>
       <c r="M31" s="52"/>
@@ -7311,7 +7467,7 @@
       <c r="BN31" s="52"/>
     </row>
     <row r="32" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A32" s="122" t="str">
+      <c r="A32" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
       </c>
@@ -7319,10 +7475,10 @@
         <v>7</v>
       </c>
       <c r="D32" s="46"/>
-      <c r="E32" s="117">
+      <c r="E32" s="116">
         <v>43129</v>
       </c>
-      <c r="F32" s="113">
+      <c r="F32" s="112">
         <f t="shared" ref="F32:F36" si="13">IF(ISBLANK(E32)," - ",IF(G32=0,E32,E32+G32-1))</f>
         <v>43129</v>
       </c>
@@ -7332,11 +7488,11 @@
       <c r="H32" s="68">
         <v>0</v>
       </c>
-      <c r="I32" s="135">
+      <c r="I32" s="134">
         <f>IF(OR(F32=0,E32=0),0,NETWORKDAYS(E32,F32))</f>
         <v>1</v>
       </c>
-      <c r="J32" s="125"/>
+      <c r="J32" s="239"/>
       <c r="K32" s="47"/>
       <c r="L32" s="47"/>
       <c r="M32" s="47"/>
@@ -7395,7 +7551,7 @@
       <c r="BN32" s="47"/>
     </row>
     <row r="33" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A33" s="122" t="str">
+      <c r="A33" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.2</v>
       </c>
@@ -7403,10 +7559,10 @@
         <v>7</v>
       </c>
       <c r="D33" s="46"/>
-      <c r="E33" s="117">
+      <c r="E33" s="116">
         <v>43130</v>
       </c>
-      <c r="F33" s="113">
+      <c r="F33" s="112">
         <f t="shared" si="13"/>
         <v>43130</v>
       </c>
@@ -7416,11 +7572,11 @@
       <c r="H33" s="68">
         <v>0</v>
       </c>
-      <c r="I33" s="135">
+      <c r="I33" s="134">
         <f>IF(OR(F33=0,E33=0),0,NETWORKDAYS(E33,F33))</f>
         <v>1</v>
       </c>
-      <c r="J33" s="125"/>
+      <c r="J33" s="241"/>
       <c r="K33" s="47"/>
       <c r="L33" s="47"/>
       <c r="M33" s="47"/>
@@ -7479,7 +7635,7 @@
       <c r="BN33" s="47"/>
     </row>
     <row r="34" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A34" s="122" t="str">
+      <c r="A34" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.3</v>
       </c>
@@ -7487,10 +7643,10 @@
         <v>7</v>
       </c>
       <c r="D34" s="46"/>
-      <c r="E34" s="117">
+      <c r="E34" s="116">
         <v>43131</v>
       </c>
-      <c r="F34" s="113">
+      <c r="F34" s="112">
         <f t="shared" si="13"/>
         <v>43131</v>
       </c>
@@ -7500,11 +7656,11 @@
       <c r="H34" s="68">
         <v>0</v>
       </c>
-      <c r="I34" s="135">
+      <c r="I34" s="134">
         <f>IF(OR(F34=0,E34=0),0,NETWORKDAYS(E34,F34))</f>
         <v>1</v>
       </c>
-      <c r="J34" s="125"/>
+      <c r="J34" s="241"/>
       <c r="K34" s="47"/>
       <c r="L34" s="47"/>
       <c r="M34" s="47"/>
@@ -7563,7 +7719,7 @@
       <c r="BN34" s="47"/>
     </row>
     <row r="35" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A35" s="122" t="str">
+      <c r="A35" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.4</v>
       </c>
@@ -7571,10 +7727,10 @@
         <v>7</v>
       </c>
       <c r="D35" s="46"/>
-      <c r="E35" s="117">
+      <c r="E35" s="116">
         <v>43132</v>
       </c>
-      <c r="F35" s="113">
+      <c r="F35" s="112">
         <f t="shared" si="13"/>
         <v>43132</v>
       </c>
@@ -7584,11 +7740,11 @@
       <c r="H35" s="68">
         <v>0</v>
       </c>
-      <c r="I35" s="135">
+      <c r="I35" s="134">
         <f>IF(OR(F35=0,E35=0),0,NETWORKDAYS(E35,F35))</f>
         <v>1</v>
       </c>
-      <c r="J35" s="125"/>
+      <c r="J35" s="241"/>
       <c r="K35" s="47"/>
       <c r="L35" s="47"/>
       <c r="M35" s="47"/>
@@ -7647,7 +7803,7 @@
       <c r="BN35" s="47"/>
     </row>
     <row r="36" spans="1:66" s="45" customFormat="1" ht="18">
-      <c r="A36" s="122" t="str">
+      <c r="A36" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.5</v>
       </c>
@@ -7655,10 +7811,10 @@
         <v>7</v>
       </c>
       <c r="D36" s="46"/>
-      <c r="E36" s="117">
+      <c r="E36" s="116">
         <v>43133</v>
       </c>
-      <c r="F36" s="113">
+      <c r="F36" s="112">
         <f t="shared" si="13"/>
         <v>43133</v>
       </c>
@@ -7668,11 +7824,11 @@
       <c r="H36" s="68">
         <v>0</v>
       </c>
-      <c r="I36" s="135">
+      <c r="I36" s="134">
         <f>IF(OR(F36=0,E36=0),0,NETWORKDAYS(E36,F36))</f>
         <v>1</v>
       </c>
-      <c r="J36" s="125"/>
+      <c r="J36" s="244"/>
       <c r="K36" s="47"/>
       <c r="L36" s="47"/>
       <c r="M36" s="47"/>
@@ -7735,12 +7891,12 @@
       <c r="B37" s="53"/>
       <c r="C37" s="53"/>
       <c r="D37" s="54"/>
-      <c r="E37" s="116"/>
-      <c r="F37" s="116"/>
+      <c r="E37" s="115"/>
+      <c r="F37" s="115"/>
       <c r="G37" s="55"/>
       <c r="H37" s="56"/>
-      <c r="I37" s="138"/>
-      <c r="J37" s="127"/>
+      <c r="I37" s="137"/>
+      <c r="J37" s="126"/>
       <c r="K37" s="47"/>
       <c r="L37" s="47"/>
       <c r="M37" s="47"/>
@@ -7803,12 +7959,12 @@
       <c r="B38" s="53"/>
       <c r="C38" s="53"/>
       <c r="D38" s="54"/>
-      <c r="E38" s="116"/>
-      <c r="F38" s="116"/>
+      <c r="E38" s="115"/>
+      <c r="F38" s="115"/>
       <c r="G38" s="55"/>
       <c r="H38" s="56"/>
-      <c r="I38" s="138"/>
-      <c r="J38" s="127"/>
+      <c r="I38" s="137"/>
+      <c r="J38" s="126"/>
       <c r="K38" s="47"/>
       <c r="L38" s="47"/>
       <c r="M38" s="47"/>
@@ -7867,18 +8023,18 @@
       <c r="BN38" s="47"/>
     </row>
     <row r="39" spans="1:66" s="58" customFormat="1" ht="27" customHeight="1" thickBot="1">
-      <c r="A39" s="139" t="s">
+      <c r="A39" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="71"/>
-      <c r="C39" s="71"/>
-      <c r="D39" s="71"/>
-      <c r="E39" s="71"/>
-      <c r="F39" s="71"/>
-      <c r="G39" s="71"/>
-      <c r="H39" s="71"/>
-      <c r="I39" s="71"/>
-      <c r="J39" s="71"/>
+      <c r="B39" s="70"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="70"/>
       <c r="K39" s="47"/>
       <c r="L39" s="47"/>
       <c r="M39" s="47"/>
@@ -7937,18 +8093,18 @@
       <c r="BN39" s="47"/>
     </row>
     <row r="40" spans="1:66" s="57" customFormat="1" ht="19" thickTop="1">
-      <c r="A40" s="140" t="s">
+      <c r="A40" s="139" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="141"/>
-      <c r="C40" s="141"/>
-      <c r="D40" s="141"/>
-      <c r="E40" s="142"/>
-      <c r="F40" s="142"/>
-      <c r="G40" s="141"/>
-      <c r="H40" s="141"/>
-      <c r="I40" s="143"/>
-      <c r="J40" s="144"/>
+      <c r="B40" s="140"/>
+      <c r="C40" s="140"/>
+      <c r="D40" s="140"/>
+      <c r="E40" s="141"/>
+      <c r="F40" s="141"/>
+      <c r="G40" s="140"/>
+      <c r="H40" s="140"/>
+      <c r="I40" s="142"/>
+      <c r="J40" s="143"/>
       <c r="K40" s="47"/>
       <c r="L40" s="47"/>
       <c r="M40" s="47"/>
@@ -8007,21 +8163,21 @@
       <c r="BN40" s="47"/>
     </row>
     <row r="41" spans="1:66" s="57" customFormat="1" ht="18">
-      <c r="A41" s="123" t="str">
+      <c r="A41" s="122" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
       </c>
-      <c r="B41" s="134" t="s">
+      <c r="B41" s="133" t="s">
         <v>62</v>
       </c>
       <c r="C41" s="43"/>
       <c r="D41" s="49"/>
-      <c r="E41" s="114"/>
-      <c r="F41" s="115"/>
+      <c r="E41" s="113"/>
+      <c r="F41" s="114"/>
       <c r="G41" s="50"/>
       <c r="H41" s="51"/>
-      <c r="I41" s="136"/>
-      <c r="J41" s="126"/>
+      <c r="I41" s="135"/>
+      <c r="J41" s="125"/>
       <c r="K41" s="47"/>
       <c r="L41" s="47"/>
       <c r="M41" s="47"/>
@@ -8080,7 +8236,7 @@
       <c r="BN41" s="47"/>
     </row>
     <row r="42" spans="1:66" s="57" customFormat="1" ht="18">
-      <c r="A42" s="122" t="str">
+      <c r="A42" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
@@ -8089,8 +8245,8 @@
       </c>
       <c r="C42" s="45"/>
       <c r="D42" s="46"/>
-      <c r="E42" s="117"/>
-      <c r="F42" s="113" t="str">
+      <c r="E42" s="116"/>
+      <c r="F42" s="112" t="str">
         <f>IF(ISBLANK(E42)," - ",IF(G42=0,E42,E42+G42-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
@@ -8098,11 +8254,11 @@
       <c r="H42" s="68">
         <v>0</v>
       </c>
-      <c r="I42" s="135">
+      <c r="I42" s="134">
         <f>IF(OR(F42=0,E42=0),0,NETWORKDAYS(E42,F42))</f>
         <v>0</v>
       </c>
-      <c r="J42" s="125"/>
+      <c r="J42" s="124"/>
       <c r="K42" s="47"/>
       <c r="L42" s="47"/>
       <c r="M42" s="47"/>
@@ -8161,7 +8317,7 @@
       <c r="BN42" s="47"/>
     </row>
     <row r="43" spans="1:66" s="57" customFormat="1" ht="18">
-      <c r="A43" s="122" t="str">
+      <c r="A43" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.1</v>
       </c>
@@ -8170,8 +8326,8 @@
       </c>
       <c r="C43" s="45"/>
       <c r="D43" s="46"/>
-      <c r="E43" s="117"/>
-      <c r="F43" s="113" t="str">
+      <c r="E43" s="116"/>
+      <c r="F43" s="112" t="str">
         <f t="shared" ref="F43:F44" si="14">IF(ISBLANK(E43)," - ",IF(G43=0,E43,E43+G43-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
@@ -8179,11 +8335,11 @@
       <c r="H43" s="68">
         <v>0</v>
       </c>
-      <c r="I43" s="135">
+      <c r="I43" s="134">
         <f t="shared" ref="I43:I44" si="15">IF(OR(F43=0,E43=0),0,NETWORKDAYS(E43,F43))</f>
         <v>0</v>
       </c>
-      <c r="J43" s="125"/>
+      <c r="J43" s="124"/>
       <c r="K43" s="47"/>
       <c r="L43" s="47"/>
       <c r="M43" s="47"/>
@@ -8242,7 +8398,7 @@
       <c r="BN43" s="47"/>
     </row>
     <row r="44" spans="1:66" s="57" customFormat="1" ht="18">
-      <c r="A44" s="122" t="str">
+      <c r="A44" s="121" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
         <v>1.1.1.1</v>
       </c>
@@ -8251,8 +8407,8 @@
       </c>
       <c r="C44" s="45"/>
       <c r="D44" s="46"/>
-      <c r="E44" s="117"/>
-      <c r="F44" s="113" t="str">
+      <c r="E44" s="116"/>
+      <c r="F44" s="112" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve"> - </v>
       </c>
@@ -8260,11 +8416,11 @@
       <c r="H44" s="68">
         <v>0</v>
       </c>
-      <c r="I44" s="135">
+      <c r="I44" s="134">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J44" s="125"/>
+      <c r="J44" s="124"/>
       <c r="K44" s="47"/>
       <c r="L44" s="47"/>
       <c r="M44" s="47"/>
@@ -8395,14 +8551,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="BH4:BN4"/>
-    <mergeCell ref="BH5:BN5"/>
-    <mergeCell ref="AM5:AS5"/>
-    <mergeCell ref="AT4:AZ4"/>
-    <mergeCell ref="AT5:AZ5"/>
-    <mergeCell ref="AM4:AS4"/>
-    <mergeCell ref="BA4:BG4"/>
-    <mergeCell ref="BA5:BG5"/>
     <mergeCell ref="AD1:AR1"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
@@ -8414,6 +8562,14 @@
     <mergeCell ref="K5:Q5"/>
     <mergeCell ref="Y4:AE4"/>
     <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="BH4:BN4"/>
+    <mergeCell ref="BH5:BN5"/>
+    <mergeCell ref="AM5:AS5"/>
+    <mergeCell ref="AT4:AZ4"/>
+    <mergeCell ref="AT5:AZ5"/>
+    <mergeCell ref="AM4:AS4"/>
+    <mergeCell ref="BA4:BG4"/>
+    <mergeCell ref="BA5:BG5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H40:H44 H8:H38">
@@ -8538,7 +8694,7 @@
       <c r="C1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="14">
-      <c r="A2" s="156" t="s">
+      <c r="A2" s="155" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="3"/>
@@ -8550,37 +8706,37 @@
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1" ht="18">
-      <c r="A4" s="157" t="s">
+      <c r="A4" s="156" t="s">
         <v>78</v>
       </c>
       <c r="B4" s="25"/>
     </row>
     <row r="5" spans="1:4" s="2" customFormat="1" ht="60">
-      <c r="B5" s="158" t="s">
+      <c r="B5" s="157" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30">
-      <c r="B7" s="158" t="s">
+      <c r="B7" s="157" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14">
-      <c r="B9" s="156" t="s">
+      <c r="B9" s="155" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30">
-      <c r="B11" s="159" t="s">
+      <c r="B11" s="158" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="13" customFormat="1"/>
     <row r="13" spans="1:4" ht="18">
-      <c r="A13" s="220" t="s">
+      <c r="A13" s="228" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="220"/>
+      <c r="B13" s="228"/>
     </row>
     <row r="14" spans="1:4" s="2" customFormat="1">
       <c r="A14" s="13"/>
@@ -8589,187 +8745,187 @@
       <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:4" s="2" customFormat="1" ht="18">
-      <c r="A15" s="160"/>
-      <c r="B15" s="161" t="s">
+      <c r="A15" s="159"/>
+      <c r="B15" s="160" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="162"/>
-      <c r="D15" s="162"/>
+      <c r="C15" s="161"/>
+      <c r="D15" s="161"/>
     </row>
     <row r="16" spans="1:4" ht="18">
-      <c r="A16" s="160"/>
-      <c r="B16" s="163" t="s">
+      <c r="A16" s="159"/>
+      <c r="B16" s="162" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="162"/>
-      <c r="D16" s="162"/>
+      <c r="C16" s="161"/>
+      <c r="D16" s="161"/>
     </row>
     <row r="17" spans="1:4" ht="18">
-      <c r="A17" s="164"/>
-      <c r="B17" s="163" t="s">
+      <c r="A17" s="163"/>
+      <c r="B17" s="162" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18">
-      <c r="A18" s="164"/>
-      <c r="B18" s="163" t="s">
+      <c r="A18" s="163"/>
+      <c r="B18" s="162" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="2" customFormat="1" ht="30">
-      <c r="A19" s="165"/>
-      <c r="B19" s="163" t="s">
+      <c r="A19" s="164"/>
+      <c r="B19" s="162" t="s">
         <v>133</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
     </row>
     <row r="20" spans="1:4" ht="18">
-      <c r="A20" s="164"/>
-      <c r="B20" s="163" t="s">
+      <c r="A20" s="163"/>
+      <c r="B20" s="162" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="2" customFormat="1" ht="18">
-      <c r="A21" s="166"/>
-      <c r="B21" s="167" t="s">
+      <c r="A21" s="165"/>
+      <c r="B21" s="166" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="2" customFormat="1" ht="18">
-      <c r="A22" s="166"/>
+      <c r="A22" s="165"/>
       <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:4" ht="18">
-      <c r="A23" s="220" t="s">
+      <c r="A23" s="228" t="s">
         <v>86</v>
       </c>
-      <c r="B23" s="220"/>
+      <c r="B23" s="228"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="45">
-      <c r="A24" s="166"/>
-      <c r="B24" s="163" t="s">
+      <c r="A24" s="165"/>
+      <c r="B24" s="162" t="s">
         <v>87</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" ht="18">
-      <c r="A25" s="166"/>
-      <c r="B25" s="163"/>
+      <c r="A25" s="165"/>
+      <c r="B25" s="162"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" ht="18">
-      <c r="A26" s="166"/>
-      <c r="B26" s="168" t="s">
+      <c r="A26" s="165"/>
+      <c r="B26" s="167" t="s">
         <v>88</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" ht="18">
-      <c r="A27" s="166"/>
-      <c r="B27" s="163" t="s">
+      <c r="A27" s="165"/>
+      <c r="B27" s="162" t="s">
         <v>89</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" ht="30">
-      <c r="A28" s="166"/>
-      <c r="B28" s="163" t="s">
+      <c r="A28" s="165"/>
+      <c r="B28" s="162" t="s">
         <v>90</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" ht="18">
-      <c r="A29" s="166"/>
-      <c r="B29" s="163"/>
+      <c r="A29" s="165"/>
+      <c r="B29" s="162"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" ht="18">
-      <c r="A30" s="166"/>
-      <c r="B30" s="168" t="s">
+      <c r="A30" s="165"/>
+      <c r="B30" s="167" t="s">
         <v>91</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" ht="18">
-      <c r="A31" s="166"/>
-      <c r="B31" s="163" t="s">
+      <c r="A31" s="165"/>
+      <c r="B31" s="162" t="s">
         <v>92</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" ht="18">
-      <c r="A32" s="166"/>
-      <c r="B32" s="163" t="s">
+      <c r="A32" s="165"/>
+      <c r="B32" s="162" t="s">
         <v>93</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" ht="18">
-      <c r="A33" s="166"/>
+      <c r="A33" s="165"/>
       <c r="B33" s="4"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" ht="30">
-      <c r="A34" s="166"/>
-      <c r="B34" s="163" t="s">
+      <c r="A34" s="165"/>
+      <c r="B34" s="162" t="s">
         <v>94</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" ht="18">
-      <c r="A35" s="166"/>
-      <c r="B35" s="169" t="s">
+      <c r="A35" s="165"/>
+      <c r="B35" s="168" t="s">
         <v>95</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" ht="18">
-      <c r="A36" s="166"/>
+      <c r="A36" s="165"/>
       <c r="B36" s="4"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" ht="18">
-      <c r="A37" s="220" t="s">
+      <c r="A37" s="228" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="220"/>
+      <c r="B37" s="228"/>
     </row>
     <row r="38" spans="1:4" ht="30">
-      <c r="B38" s="163" t="s">
+      <c r="B38" s="162" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15">
-      <c r="B40" s="163" t="s">
+      <c r="B40" s="162" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="2" customFormat="1" ht="30">
       <c r="A42" s="13"/>
-      <c r="B42" s="163" t="s">
+      <c r="B42" s="162" t="s">
         <v>98</v>
       </c>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
     </row>
     <row r="44" spans="1:4" ht="30">
-      <c r="B44" s="163" t="s">
+      <c r="B44" s="162" t="s">
         <v>99</v>
       </c>
     </row>
@@ -8777,7 +8933,7 @@
       <c r="B45" s="14"/>
     </row>
     <row r="46" spans="1:4" ht="30">
-      <c r="B46" s="163" t="s">
+      <c r="B46" s="162" t="s">
         <v>100</v>
       </c>
     </row>
@@ -8785,13 +8941,13 @@
       <c r="B47" s="6"/>
     </row>
     <row r="48" spans="1:4" ht="18">
-      <c r="A48" s="220" t="s">
+      <c r="A48" s="228" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="220"/>
+      <c r="B48" s="228"/>
     </row>
     <row r="49" spans="1:2" ht="30">
-      <c r="B49" s="163" t="s">
+      <c r="B49" s="162" t="s">
         <v>101</v>
       </c>
     </row>
@@ -8799,86 +8955,86 @@
       <c r="B50" s="6"/>
     </row>
     <row r="51" spans="1:2" ht="15">
-      <c r="A51" s="170" t="s">
+      <c r="A51" s="169" t="s">
         <v>10</v>
       </c>
-      <c r="B51" s="163" t="s">
+      <c r="B51" s="162" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15">
-      <c r="A52" s="170" t="s">
+      <c r="A52" s="169" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="163" t="s">
+      <c r="B52" s="162" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15">
-      <c r="A53" s="170" t="s">
+      <c r="A53" s="169" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="163" t="s">
+      <c r="B53" s="162" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="30">
-      <c r="A54" s="159"/>
-      <c r="B54" s="163" t="s">
+      <c r="A54" s="158"/>
+      <c r="B54" s="162" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="30">
-      <c r="A55" s="159"/>
-      <c r="B55" s="163" t="s">
+      <c r="A55" s="158"/>
+      <c r="B55" s="162" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15">
-      <c r="A56" s="170" t="s">
+      <c r="A56" s="169" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="163" t="s">
+      <c r="B56" s="162" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15">
-      <c r="A57" s="159"/>
-      <c r="B57" s="163" t="s">
+      <c r="A57" s="158"/>
+      <c r="B57" s="162" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:2" s="13" customFormat="1" ht="15">
-      <c r="A58" s="159"/>
-      <c r="B58" s="163" t="s">
+      <c r="A58" s="158"/>
+      <c r="B58" s="162" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:2" s="13" customFormat="1" ht="15">
-      <c r="A59" s="170" t="s">
+      <c r="A59" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="163" t="s">
+      <c r="B59" s="162" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:2" s="13" customFormat="1" ht="30">
-      <c r="A60" s="159"/>
-      <c r="B60" s="163" t="s">
+      <c r="A60" s="158"/>
+      <c r="B60" s="162" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15">
-      <c r="A61" s="170" t="s">
+      <c r="A61" s="169" t="s">
         <v>107</v>
       </c>
-      <c r="B61" s="163" t="s">
+      <c r="B61" s="162" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:2" s="13" customFormat="1" ht="15">
-      <c r="A62" s="171"/>
-      <c r="B62" s="163" t="s">
+      <c r="A62" s="170"/>
+      <c r="B62" s="162" t="s">
         <v>109</v>
       </c>
     </row>
@@ -8886,14 +9042,14 @@
       <c r="B63" s="5"/>
     </row>
     <row r="64" spans="1:2" s="13" customFormat="1" ht="18">
-      <c r="A64" s="220" t="s">
+      <c r="A64" s="228" t="s">
         <v>8</v>
       </c>
-      <c r="B64" s="220"/>
+      <c r="B64" s="228"/>
     </row>
     <row r="65" spans="1:4" s="2" customFormat="1" ht="45">
       <c r="A65" s="13"/>
-      <c r="B65" s="163" t="s">
+      <c r="B65" s="162" t="s">
         <v>110</v>
       </c>
       <c r="C65" s="13"/>
@@ -8903,172 +9059,172 @@
       <c r="B66" s="6"/>
     </row>
     <row r="67" spans="1:4" s="2" customFormat="1" ht="18">
-      <c r="A67" s="220" t="s">
+      <c r="A67" s="228" t="s">
         <v>3</v>
       </c>
-      <c r="B67" s="220"/>
+      <c r="B67" s="228"/>
     </row>
     <row r="68" spans="1:4" s="2" customFormat="1" ht="15">
-      <c r="A68" s="172" t="s">
+      <c r="A68" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="B68" s="173" t="s">
+      <c r="B68" s="172" t="s">
         <v>111</v>
       </c>
       <c r="C68" s="13"/>
       <c r="D68" s="13"/>
     </row>
     <row r="69" spans="1:4" ht="30">
-      <c r="A69" s="174"/>
-      <c r="B69" s="175" t="s">
+      <c r="A69" s="173"/>
+      <c r="B69" s="174" t="s">
         <v>112</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" s="2" customFormat="1" ht="14">
-      <c r="A70" s="174"/>
-      <c r="B70" s="176"/>
+      <c r="A70" s="173"/>
+      <c r="B70" s="175"/>
     </row>
     <row r="71" spans="1:4" s="2" customFormat="1" ht="15">
-      <c r="A71" s="172" t="s">
+      <c r="A71" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="B71" s="173" t="s">
+      <c r="B71" s="172" t="s">
         <v>113</v>
       </c>
       <c r="C71" s="13"/>
       <c r="D71" s="13"/>
     </row>
     <row r="72" spans="1:4" s="2" customFormat="1" ht="30">
-      <c r="A72" s="174"/>
-      <c r="B72" s="175" t="s">
+      <c r="A72" s="173"/>
+      <c r="B72" s="174" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="2" customFormat="1" ht="14">
-      <c r="A73" s="174"/>
-      <c r="B73" s="176"/>
+      <c r="A73" s="173"/>
+      <c r="B73" s="175"/>
     </row>
     <row r="74" spans="1:4" ht="14">
-      <c r="A74" s="172" t="s">
+      <c r="A74" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="B74" s="177" t="s">
+      <c r="B74" s="176" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="30">
-      <c r="A75" s="174"/>
-      <c r="B75" s="158" t="s">
+      <c r="A75" s="173"/>
+      <c r="B75" s="157" t="s">
         <v>116</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4" s="2" customFormat="1" ht="14">
-      <c r="A76" s="171"/>
-      <c r="B76" s="171"/>
+      <c r="A76" s="170"/>
+      <c r="B76" s="170"/>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
     </row>
     <row r="77" spans="1:4" s="2" customFormat="1" ht="14">
-      <c r="A77" s="172" t="s">
+      <c r="A77" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="B77" s="177" t="s">
+      <c r="B77" s="176" t="s">
         <v>117</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
     </row>
     <row r="78" spans="1:4" s="2" customFormat="1" ht="30">
-      <c r="A78" s="174"/>
-      <c r="B78" s="158" t="s">
+      <c r="A78" s="173"/>
+      <c r="B78" s="157" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="14">
-      <c r="A79" s="171"/>
-      <c r="B79" s="171"/>
+      <c r="A79" s="170"/>
+      <c r="B79" s="170"/>
     </row>
     <row r="80" spans="1:4" ht="14">
-      <c r="A80" s="172" t="s">
+      <c r="A80" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="B80" s="177" t="s">
+      <c r="B80" s="176" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="81" spans="1:4" s="2" customFormat="1" ht="15">
-      <c r="A81" s="174"/>
-      <c r="B81" s="178" t="s">
+      <c r="A81" s="173"/>
+      <c r="B81" s="177" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="82" spans="1:4" s="2" customFormat="1" ht="15">
-      <c r="A82" s="174"/>
-      <c r="B82" s="178" t="s">
+      <c r="A82" s="173"/>
+      <c r="B82" s="177" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="83" spans="1:4" s="2" customFormat="1" ht="15">
-      <c r="A83" s="174"/>
-      <c r="B83" s="178" t="s">
+      <c r="A83" s="173"/>
+      <c r="B83" s="177" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="14">
-      <c r="A84" s="171"/>
-      <c r="B84" s="179"/>
+      <c r="A84" s="170"/>
+      <c r="B84" s="178"/>
     </row>
     <row r="85" spans="1:4" ht="14">
-      <c r="A85" s="172" t="s">
+      <c r="A85" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="B85" s="177" t="s">
+      <c r="B85" s="176" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="45">
-      <c r="A86" s="174"/>
-      <c r="B86" s="158" t="s">
+      <c r="A86" s="173"/>
+      <c r="B86" s="157" t="s">
         <v>124</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
     </row>
     <row r="87" spans="1:4" ht="15">
-      <c r="A87" s="174"/>
-      <c r="B87" s="180" t="s">
+      <c r="A87" s="173"/>
+      <c r="B87" s="179" t="s">
         <v>125</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
     </row>
     <row r="88" spans="1:4" ht="45">
-      <c r="A88" s="174"/>
-      <c r="B88" s="181" t="s">
+      <c r="A88" s="173"/>
+      <c r="B88" s="180" t="s">
         <v>126</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
     <row r="89" spans="1:4" ht="14">
-      <c r="A89" s="171"/>
-      <c r="B89" s="171"/>
+      <c r="A89" s="170"/>
+      <c r="B89" s="170"/>
     </row>
     <row r="90" spans="1:4" ht="14">
-      <c r="A90" s="172" t="s">
+      <c r="A90" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="B90" s="182" t="s">
+      <c r="B90" s="181" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="30">
-      <c r="A91" s="159"/>
-      <c r="B91" s="178" t="s">
+      <c r="A91" s="158"/>
+      <c r="B91" s="177" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>